<commit_message>
added image on home page
</commit_message>
<xml_diff>
--- a/Task List.xlsx
+++ b/Task List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Develop\food-delivery-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F9850A-BE74-45D2-8B29-ED14C8613438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156C2C66-5366-4451-9327-1F3245CDCFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>Task Name</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>Redux</t>
-  </si>
-  <si>
-    <t>Check which Redux livrary to use. Learn the differences and advantages.</t>
   </si>
   <si>
     <t>Comments</t>
@@ -112,6 +109,21 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Material UI</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Check which Redux library to use. Learn the differences and advantages.</t>
+  </si>
+  <si>
+    <t>Add restaurants after the image.</t>
   </si>
 </sst>
 </file>
@@ -171,7 +183,28 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
       <border>
@@ -217,28 +250,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="4" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
       <border>
@@ -711,7 +723,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,7 +758,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -760,7 +772,6 @@
         <v>11</v>
       </c>
       <c r="D2" s="2">
-        <f ca="1">TODAY()</f>
         <v>44996</v>
       </c>
     </row>
@@ -772,11 +783,16 @@
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2">
-        <f ca="1">TODAY()</f>
         <v>44996</v>
+      </c>
+      <c r="E3" s="2">
+        <v>44997</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -784,15 +800,12 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2">
-        <f ca="1">TODAY()</f>
-        <v>44996</v>
-      </c>
+      <c r="D4" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:F4">
@@ -831,10 +844,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275D0864-C0D6-4562-9FF2-7C7C07019602}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -866,15 +879,15 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -886,10 +899,10 @@
     </row>
     <row r="3" spans="1:7" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -901,18 +914,35 @@
     </row>
     <row r="4" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="D4" s="2">
+        <v>44996</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:F4">
@@ -925,17 +955,17 @@
       <formula>$C3="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:G4">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A2:G5">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$C2="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$C2="Testing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>$C2="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>$C2="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added basic navbar structure.
</commit_message>
<xml_diff>
--- a/Task List.xlsx
+++ b/Task List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Develop\food-delivery-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0463E599-B60E-40E3-B900-D53C22199B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA15A4E-5D61-4369-A316-D74FF1C00FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HLD" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Task Name</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Create a global CSS structure</t>
+  </si>
+  <si>
+    <t>Navbar list</t>
+  </si>
+  <si>
+    <t>Write minimal to show content in Navbar</t>
   </si>
 </sst>
 </file>
@@ -188,7 +194,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="17">
     <dxf>
       <fill>
         <patternFill>
@@ -303,6 +309,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="4" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -326,7 +353,28 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
       <border>
@@ -349,28 +397,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
       <border>
@@ -414,27 +441,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="4" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -458,28 +464,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
       <border>
@@ -502,29 +487,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -546,206 +508,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
       <border>
@@ -1085,7 +848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1186,47 +949,47 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:F4">
-    <cfRule type="expression" dxfId="21" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="10" stopIfTrue="1">
       <formula>$C4="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:F3">
-    <cfRule type="expression" dxfId="20" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="9" stopIfTrue="1">
       <formula>$C3="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:G4">
-    <cfRule type="expression" dxfId="19" priority="8">
+    <cfRule type="expression" dxfId="14" priority="8">
       <formula>$C2="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="12">
+    <cfRule type="expression" dxfId="13" priority="12">
       <formula>$C2="Not Started"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="7">
+    <cfRule type="expression" dxfId="12" priority="7">
       <formula>$C2="Testing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="6">
+    <cfRule type="expression" dxfId="11" priority="6">
       <formula>$C2="In Progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="15" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="4" stopIfTrue="1">
       <formula>$C5="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>$C5="Testing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="3">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>$C5="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>$C5="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:C5">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$C5="In Progress"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1242,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275D0864-C0D6-4562-9FF2-7C7C07019602}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1342,28 +1105,39 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A4:F4">
-    <cfRule type="expression" dxfId="27" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>$C4="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:F3">
-    <cfRule type="expression" dxfId="26" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>$C3="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:G5">
-    <cfRule type="expression" dxfId="25" priority="1">
+  <conditionalFormatting sqref="A2:G5 A6:C6">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$C2="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$C2="Testing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>$C2="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="6">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>$C2="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added validaion in login and signup forms
</commit_message>
<xml_diff>
--- a/Task List.xlsx
+++ b/Task List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Develop\food-delivery-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA15A4E-5D61-4369-A316-D74FF1C00FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E474ED9-92DA-460A-9D9C-6A9FEB3EFB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Task Name</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>First glance</t>
-  </si>
-  <si>
-    <t>Add a background image , food related. Place a search bar on top of it. Search for restaurants, maybe.</t>
   </si>
   <si>
     <t>Footer</t>
@@ -138,7 +135,16 @@
     <t>Navbar list</t>
   </si>
   <si>
-    <t>Write minimal to show content in Navbar</t>
+    <t>Write minimal code to show content in Navbar</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>Add input field validation in login and signup form</t>
+  </si>
+  <si>
+    <t>Add a background image , food related.</t>
   </si>
 </sst>
 </file>
@@ -182,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -190,6 +196,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -895,13 +902,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2">
         <v>44996</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -912,7 +919,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2">
         <v>44996</v>
@@ -921,7 +928,7 @@
         <v>44997</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -929,7 +936,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -938,10 +945,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
@@ -1005,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275D0864-C0D6-4562-9FF2-7C7C07019602}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1017,6 +1024,7 @@
     <col min="2" max="2" width="48.6640625" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1048,10 +1056,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
@@ -1060,10 +1068,10 @@
     </row>
     <row r="3" spans="1:7" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -1075,10 +1083,10 @@
     </row>
     <row r="4" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -1086,16 +1094,18 @@
       <c r="D4" s="2">
         <v>44996</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="2">
+        <v>45003</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
@@ -1105,15 +1115,32 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3">
+        <v>45003</v>
+      </c>
+      <c r="E7" s="3">
+        <v>45004</v>
       </c>
     </row>
   </sheetData>
@@ -1127,7 +1154,7 @@
       <formula>$C3="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:G5 A6:C6">
+  <conditionalFormatting sqref="A2:G5 A6:C7">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>$C2="In Progress"</formula>
     </cfRule>

</xml_diff>

<commit_message>
refactored authentication modal, routes and controllers
</commit_message>
<xml_diff>
--- a/Task List.xlsx
+++ b/Task List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Develop\food-delivery-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05973D65-2536-4863-9A49-CD85AFA8D002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8262E298-0FE2-4F4D-9E8C-AF03ECCFD259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HLD" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <si>
     <t>Task Name</t>
   </si>
@@ -168,6 +168,24 @@
   </si>
   <si>
     <t>Create a sign up form</t>
+  </si>
+  <si>
+    <t>Login form</t>
+  </si>
+  <si>
+    <t>Create a login form</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Redirect</t>
+  </si>
+  <si>
+    <t>After signup, tell user to login. On login check if the token is valid and then redirect to registration page. If token is not valid, redirect to login page</t>
+  </si>
+  <si>
+    <t>Design</t>
   </si>
 </sst>
 </file>
@@ -224,7 +242,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="25">
     <dxf>
       <fill>
         <patternFill>
@@ -334,159 +352,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -944,6 +809,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>74295</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39C985C2-348A-D5AA-DDCC-370FDE4689BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9951720" y="182880"/>
+          <a:ext cx="6772275" cy="5915025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1312,40 +1232,40 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C5">
-    <cfRule type="expression" dxfId="31" priority="1">
+    <cfRule type="expression" dxfId="24" priority="1">
       <formula>$C5="In Progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:F4">
-    <cfRule type="expression" dxfId="30" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="9" stopIfTrue="1">
       <formula>$C3="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:G4">
-    <cfRule type="expression" dxfId="29" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>$C2="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="7">
+    <cfRule type="expression" dxfId="21" priority="7">
       <formula>$C2="Testing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="8">
+    <cfRule type="expression" dxfId="20" priority="8">
       <formula>$C2="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="12">
+    <cfRule type="expression" dxfId="19" priority="12">
       <formula>$C2="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="25" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>$C5="Testing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="3">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>$C5="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="4" stopIfTrue="1">
       <formula>$C5="Not Started"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="5">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>$C5="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1497,21 +1417,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:C7 A2:G5">
-    <cfRule type="expression" dxfId="21" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>$C2="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>$C2="Testing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>$C2="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="6">
+    <cfRule type="expression" dxfId="11" priority="6">
       <formula>$C2="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:F4">
-    <cfRule type="expression" dxfId="17" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="4" stopIfTrue="1">
       <formula>$C3="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1529,8 +1449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABA8617-5EB2-4A42-88F4-EDE79E4B6BEE}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1575,29 +1495,45 @@
         <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2">
-        <v>45017</v>
+        <v>45018</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2"/>
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45018</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
+    <row r="4" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45019</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1626,21 +1562,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:C7 A2:G5">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>$C2="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>$C2="Testing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$C2="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>$C2="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:F4">
-    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
       <formula>$C3="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1655,10 +1591,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4086CAA4-A751-449E-A70D-7B7A8B6068E4}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1669,9 +1605,10 @@
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.77734375" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1693,8 +1630,11 @@
       <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -1711,7 +1651,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -1728,7 +1668,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1737,7 +1677,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1746,12 +1686,12 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1760,21 +1700,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:C7 A4:G5">
-    <cfRule type="expression" dxfId="16" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$C4="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$C4="Testing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$C4="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="6">
+    <cfRule type="expression" dxfId="1" priority="6">
       <formula>$C4="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:F4">
-    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="5" stopIfTrue="1">
       <formula>$C4="Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1784,5 +1724,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>